<commit_message>
version completa final 2
</commit_message>
<xml_diff>
--- a/TP Final - Testing/ClinicaCajaBlanca.xlsx
+++ b/TP Final - Testing/ClinicaCajaBlanca.xlsx
@@ -215,7 +215,7 @@
 listaDeInsumos = {}</t>
   </si>
   <si>
-    <t>numeroDeFactura = 1, fechaDeSolicitud = 25/10/2010,
+    <t>numeroDeFactura = 1, fechaDeSolicitud = 25/11/2010,
 listaDeInsumos = {100}</t>
   </si>
   <si>
@@ -489,7 +489,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -566,6 +566,9 @@
     <xf borderId="2" fillId="10" fontId="12" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
+    <xf borderId="2" fillId="10" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
@@ -584,13 +587,13 @@
     <xf borderId="2" fillId="9" fontId="12" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="2" fillId="10" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="9" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="10" fillId="10" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="9" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="10" fillId="10" fontId="13" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="10" fillId="9" fontId="13" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1361,11 +1364,11 @@
       <c r="E120" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="F120" s="34">
-        <v>0.0</v>
-      </c>
-      <c r="G120" s="34">
-        <v>0.0</v>
+      <c r="F120" s="36">
+        <v>200.0</v>
+      </c>
+      <c r="G120" s="36">
+        <v>200.0</v>
       </c>
     </row>
     <row r="121" ht="15.75" customHeight="1">
@@ -1386,13 +1389,13 @@
       </c>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="E122" s="36"/>
+      <c r="E122" s="37"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="E123" s="36"/>
+      <c r="E123" s="37"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="E124" s="36"/>
+      <c r="E124" s="37"/>
     </row>
     <row r="125" ht="15.75" customHeight="1">
       <c r="A125" s="21" t="s">
@@ -1403,7 +1406,7 @@
       </c>
       <c r="C125" s="23"/>
       <c r="D125" s="23"/>
-      <c r="E125" s="37"/>
+      <c r="E125" s="38"/>
       <c r="F125" s="23"/>
       <c r="G125" s="24"/>
     </row>
@@ -1412,7 +1415,7 @@
       <c r="B126" s="33"/>
       <c r="C126" s="19"/>
       <c r="D126" s="19"/>
-      <c r="E126" s="38"/>
+      <c r="E126" s="39"/>
       <c r="F126" s="19"/>
       <c r="G126" s="20"/>
     </row>
@@ -1425,7 +1428,7 @@
       <c r="D127" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="E127" s="39" t="s">
+      <c r="E127" s="40" t="s">
         <v>41</v>
       </c>
       <c r="F127" s="26" t="s">
@@ -1477,38 +1480,38 @@
       <c r="C130" s="29">
         <v>9.0</v>
       </c>
-      <c r="D130" s="40" t="s">
+      <c r="D130" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="E130" s="41" t="s">
+      <c r="E130" s="42" t="s">
         <v>62</v>
       </c>
       <c r="F130" s="29">
         <v>520.0</v>
       </c>
-      <c r="G130" s="29">
-        <v>660.0</v>
+      <c r="G130" s="41">
+        <v>520.0</v>
       </c>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="C131" s="42">
+      <c r="C131" s="43">
         <v>10.0</v>
       </c>
-      <c r="D131" s="43" t="s">
+      <c r="D131" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="E131" s="44" t="s">
+      <c r="E131" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="F131" s="43">
+      <c r="F131" s="44">
         <v>760.0</v>
       </c>
-      <c r="G131" s="43">
-        <v>760.0</v>
+      <c r="G131" s="44">
+        <v>620.0</v>
       </c>
     </row>
     <row r="132" ht="15.75" customHeight="1">
-      <c r="E132" s="36"/>
+      <c r="E132" s="37"/>
     </row>
     <row r="133" ht="15.75" customHeight="1">
       <c r="A133" s="21" t="s">
@@ -1519,7 +1522,7 @@
       </c>
       <c r="C133" s="23"/>
       <c r="D133" s="23"/>
-      <c r="E133" s="37"/>
+      <c r="E133" s="38"/>
       <c r="F133" s="23"/>
       <c r="G133" s="24"/>
     </row>
@@ -1528,7 +1531,7 @@
       <c r="B134" s="33"/>
       <c r="C134" s="19"/>
       <c r="D134" s="19"/>
-      <c r="E134" s="38"/>
+      <c r="E134" s="39"/>
       <c r="F134" s="19"/>
       <c r="G134" s="20"/>
     </row>
@@ -1541,7 +1544,7 @@
       <c r="D135" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="E135" s="39" t="s">
+      <c r="E135" s="40" t="s">
         <v>41</v>
       </c>
       <c r="F135" s="26" t="s">
@@ -1571,20 +1574,20 @@
       </c>
     </row>
     <row r="137" ht="15.75" customHeight="1">
-      <c r="C137" s="29">
+      <c r="C137" s="36">
         <v>12.0</v>
       </c>
-      <c r="D137" s="29" t="s">
+      <c r="D137" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="E137" s="41" t="s">
+      <c r="E137" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="F137" s="29">
+      <c r="F137" s="36">
         <v>340.0</v>
       </c>
-      <c r="G137" s="29">
-        <v>420.0</v>
+      <c r="G137" s="36">
+        <v>340.0</v>
       </c>
     </row>
     <row r="138" ht="15.75" customHeight="1">
@@ -1605,7 +1608,7 @@
       </c>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="E139" s="36"/>
+      <c r="E139" s="37"/>
     </row>
     <row r="140" ht="15.75" customHeight="1">
       <c r="A140" s="21" t="s">
@@ -1616,7 +1619,7 @@
       </c>
       <c r="C140" s="23"/>
       <c r="D140" s="23"/>
-      <c r="E140" s="37"/>
+      <c r="E140" s="38"/>
       <c r="F140" s="23"/>
       <c r="G140" s="24"/>
     </row>
@@ -1625,7 +1628,7 @@
       <c r="B141" s="33"/>
       <c r="C141" s="19"/>
       <c r="D141" s="19"/>
-      <c r="E141" s="38"/>
+      <c r="E141" s="39"/>
       <c r="F141" s="19"/>
       <c r="G141" s="20"/>
     </row>
@@ -1638,7 +1641,7 @@
       <c r="D142" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="E142" s="39" t="s">
+      <c r="E142" s="40" t="s">
         <v>41</v>
       </c>
       <c r="F142" s="26" t="s">
@@ -1660,8 +1663,8 @@
       <c r="E143" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="F143" s="34">
-        <v>0.0</v>
+      <c r="F143" s="36">
+        <v>300.0</v>
       </c>
       <c r="G143" s="34">
         <v>0.0</v>

</xml_diff>